<commit_message>
Upload initial formal budget
</commit_message>
<xml_diff>
--- a/proposal/budget.xlsx
+++ b/proposal/budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - GE\Documents\University of Pretoria\Modules\Year 4 Semester 1\EPR 402\Project budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - GE\Documents\University of Pretoria\Modules\Year 4 Semester 1\EPR 402\2021_conroy_ch\proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20D85C4-F45A-4BC9-B830-02D04EDD7CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0ABE20-3269-4276-839C-A9AB99D1FC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1920" yWindow="465" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Be Purchased" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Item description</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>Switch-mode power supply - 12V 20A</t>
+  </si>
+  <si>
+    <t>Machine Vision Camera</t>
   </si>
 </sst>
 </file>
@@ -550,8 +553,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C10" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A4:C10" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C11" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A4:C11" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -830,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,14 +1215,14 @@
         <v>43</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17" s="4">
         <v>9.9499999999999993</v>
       </c>
       <c r="H17" s="4">
         <f>PRODUCT(F17:G17)</f>
-        <v>29.849999999999998</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>44</v>
@@ -1297,10 +1300,14 @@
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="4">
+        <v>60</v>
+      </c>
+      <c r="H20" s="4">
+        <f>PRODUCT(F20:G20)</f>
         <v>60</v>
       </c>
       <c r="I20" s="9" t="s">
@@ -1326,7 +1333,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="4">
-        <f>PRODUCT(F21:G21)</f>
+        <f t="shared" ref="H21:H26" si="1">PRODUCT(F21:G21)</f>
         <v>30</v>
       </c>
       <c r="I21" s="3"/>
@@ -1354,7 +1361,7 @@
         <v>137.15</v>
       </c>
       <c r="H22" s="4">
-        <f>PRODUCT(F22:G22)</f>
+        <f t="shared" si="1"/>
         <v>137.15</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -1384,7 +1391,7 @@
         <v>114.63</v>
       </c>
       <c r="H23" s="4">
-        <f>PRODUCT(F23:G23)</f>
+        <f t="shared" si="1"/>
         <v>114.63</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -1414,7 +1421,7 @@
         <v>242.39</v>
       </c>
       <c r="H24" s="4">
-        <f>PRODUCT(F24:G24)</f>
+        <f t="shared" si="1"/>
         <v>242.39</v>
       </c>
       <c r="I24" s="5" t="s">
@@ -1442,7 +1449,7 @@
         <v>349</v>
       </c>
       <c r="H25" s="4">
-        <f>PRODUCT(F25:G25)</f>
+        <f t="shared" si="1"/>
         <v>349</v>
       </c>
       <c r="I25" s="5" t="s">
@@ -1468,7 +1475,7 @@
         <v>200</v>
       </c>
       <c r="H26" s="4">
-        <f>PRODUCT(F26:G26)</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="I26" s="5" t="s">
@@ -1487,7 +1494,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4">
         <f>SUBTOTAL(109,Table2[Overall price])</f>
-        <v>3449.07</v>
+        <v>3519.0200000000004</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -1511,7 +1518,7 @@
     <hyperlink ref="I17" r:id="rId16" xr:uid="{E61937CC-C61C-470A-888E-22589590AA4C}"/>
     <hyperlink ref="I25" r:id="rId17" xr:uid="{1DF0B828-FEFB-4DE4-88C8-0D95E6ADC11E}"/>
     <hyperlink ref="I26" r:id="rId18" xr:uid="{92BC8783-EFB5-4E77-87BC-CC8EFF783D42}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{4DAACDAD-47E0-46BD-8002-571830A20781}"/>
+    <hyperlink ref="I20" r:id="rId19" xr:uid="{7381FD2B-B8A5-4F72-94E1-FB50D814874D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
@@ -1523,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E588218-957E-4AA9-A72D-F3B084945E29}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,6 +1630,17 @@
         <v>67</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update component bank requirements in draft budget
</commit_message>
<xml_diff>
--- a/proposal/budget.xlsx
+++ b/proposal/budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - GE\Documents\University of Pretoria\Modules\Year 4 Semester 1\EPR 402\2021_conroy_ch\proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0ABE20-3269-4276-839C-A9AB99D1FC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E11A9-DBED-4AD7-9C01-19CE61E47886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1920" yWindow="465" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Be Purchased" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Item description</t>
   </si>
@@ -235,18 +235,9 @@
     <t>Wantai Stepper Motor 42BYGHW609, NEMA17, 1.8 deg/step</t>
   </si>
   <si>
-    <t>Stepper Motors</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
-    <t>Stepper Motor Drivers</t>
-  </si>
-  <si>
-    <t>Servo Motor</t>
-  </si>
-  <si>
     <t>JLC PCB</t>
   </si>
   <si>
@@ -295,7 +286,19 @@
     <t>Switch-mode power supply - 12V 20A</t>
   </si>
   <si>
-    <t>Machine Vision Camera</t>
+    <t>Logitech c920 HD webcam</t>
+  </si>
+  <si>
+    <t>Wantai Stepper Motor 20BYGH406, NEMA8, 1.8 deg/step</t>
+  </si>
+  <si>
+    <t>Wantai Dual Shaft Stepper Motor 42BYGHW920L21B2, NEMA17, 1.8 deg/step</t>
+  </si>
+  <si>
+    <t>Wantai Stepper Motor 35BYG312P1,NEMA14, 1.8 deg/step</t>
+  </si>
+  <si>
+    <t>DS3115MG Servo</t>
   </si>
 </sst>
 </file>
@@ -418,6 +421,24 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -426,27 +447,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -455,37 +455,40 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -536,33 +539,33 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5CB77036-6EDC-4C6E-AA7A-A24A28E76F4C}" name="Item description" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FCAC24A4-9102-4758-9937-C980D10B8D1D}" name="Manufacturer" dataDxfId="16" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{52A05EA1-8300-4387-B125-D38875D97D8E}" name="Manufacturer model number" dataDxfId="15" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{ECE27936-736C-4CFF-A647-CD71A598E679}" name="Store" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{4AF6CAD2-FC5A-465A-B729-4B3E153A6B59}" name="Availability" dataDxfId="13" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{CACCC691-E59B-4854-9A69-C610500DA6C2}" name="Quantity" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{40077FE9-E87F-44AF-ACCB-DC4EF8B152B1}" name="Unit price" dataDxfId="11" totalsRowDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{8E3C7A3D-5684-421B-9B35-B72A3E3493EB}" name="Overall price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{5CB77036-6EDC-4C6E-AA7A-A24A28E76F4C}" name="Item description" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{FCAC24A4-9102-4758-9937-C980D10B8D1D}" name="Manufacturer" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{52A05EA1-8300-4387-B125-D38875D97D8E}" name="Manufacturer model number" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{ECE27936-736C-4CFF-A647-CD71A598E679}" name="Store" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{4AF6CAD2-FC5A-465A-B729-4B3E153A6B59}" name="Availability" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{CACCC691-E59B-4854-9A69-C610500DA6C2}" name="Quantity" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{40077FE9-E87F-44AF-ACCB-DC4EF8B152B1}" name="Unit price" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{8E3C7A3D-5684-421B-9B35-B72A3E3493EB}" name="Overall price" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>PRODUCT(F5:G5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A381D153-A3F4-4955-9FC0-F2A8E888F576}" name="Source link" dataDxfId="9" totalsRowDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{A381D153-A3F4-4955-9FC0-F2A8E888F576}" name="Source link" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C11" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A4:C11" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A4:C13" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -833,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,13 +1233,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>39</v>
@@ -1255,17 +1258,17 @@
         <v>19.95</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>34</v>
@@ -1281,21 +1284,21 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" t="s">
         <v>80</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
@@ -1311,7 +1314,7 @@
         <v>60</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1463,10 +1466,10 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
@@ -1479,7 +1482,7 @@
         <v>200</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1530,15 +1533,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E588218-957E-4AA9-A72D-F3B084945E29}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="67.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -1599,46 +1602,68 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update draft and formal budgets
</commit_message>
<xml_diff>
--- a/proposal/budget.xlsx
+++ b/proposal/budget.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - GE\Documents\University of Pretoria\Modules\Year 4 Semester 1\EPR 402\2021_conroy_ch\proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02E11A9-DBED-4AD7-9C01-19CE61E47886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42776AC1-9134-4A04-827B-593067993FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="To Be Purchased" sheetId="1" r:id="rId1"/>
+    <sheet name="To Be Purchased" sheetId="3" r:id="rId1"/>
     <sheet name="Component Bank" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
   <si>
     <t>Item description</t>
   </si>
@@ -52,21 +52,12 @@
     <t>Source link</t>
   </si>
   <si>
-    <t>20 x 20mm Aluminium V-Slot Profile</t>
-  </si>
-  <si>
-    <t>20 x 40mm Aluminium V-Slot Profile</t>
-  </si>
-  <si>
     <t>V-Slot Wheel Kit, Solid, Delrin</t>
   </si>
   <si>
     <t>Eccentric Nut for V-Wheels</t>
   </si>
   <si>
-    <t>Timing Belt, GT2, 6mm wide, 1m long, Polyurethane</t>
-  </si>
-  <si>
     <t>Lead Screw, 8mm, Length: 300mm</t>
   </si>
   <si>
@@ -100,18 +91,6 @@
     <t>https://za.rs-online.com/web/p/products/8368941/</t>
   </si>
   <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/20-x-20mm-aluminium-v-slot-profile.html</t>
-  </si>
-  <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/20-x-40mm-aluminium-v-slot-profile.html</t>
-  </si>
-  <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/linear-chromed-steel-rod-8mm-350mm.html</t>
-  </si>
-  <si>
-    <t>https://www.diyelectronics.co.za/store/rod-end-bearings/1667-8mm-pillow-block-bearing-kp08.html</t>
-  </si>
-  <si>
     <t>https://www.3dprintingstore.co.za/centurionstore/v-slot-wheel-kit-solid-delrin.html</t>
   </si>
   <si>
@@ -121,15 +100,6 @@
     <t>https://www.3dprintingstore.co.za/centurionstore/lead-screw-8mm-length-300mm.html</t>
   </si>
   <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/flanged-nut-for-8mm-lead-screw-delrin-2mm-pitch.html</t>
-  </si>
-  <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/flexible-coupling-clamping-type.html</t>
-  </si>
-  <si>
-    <t>https://www.diyelectronics.co.za/store/pulleys/1047-mxl-pulley-8mm-bore-20-tooth-635mm-belt.html</t>
-  </si>
-  <si>
     <t>https://www.3dprintingstore.co.za/centurionstore/idler-pulley-for-6mm-belt.html</t>
   </si>
   <si>
@@ -142,9 +112,6 @@
     <t>Available</t>
   </si>
   <si>
-    <t>2-3 workings days delivery</t>
-  </si>
-  <si>
     <t>Purchased</t>
   </si>
   <si>
@@ -184,9 +151,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Components to be Purchased</t>
-  </si>
-  <si>
     <t>Project Budget</t>
   </si>
   <si>
@@ -199,21 +163,6 @@
     <t>Animal Kingdom Pet Shop</t>
   </si>
   <si>
-    <t>MXL Pulley (8mm Bore, 20 Tooth / 6.35mm Belt)</t>
-  </si>
-  <si>
-    <t>Linear Chromed Steel Rod, 8mm, 350mm</t>
-  </si>
-  <si>
-    <t>8mm Pillow Block Bearing - KP08</t>
-  </si>
-  <si>
-    <t>Flanged Nut for 8mm Lead Screw, Delrin, 2mm Pitch</t>
-  </si>
-  <si>
-    <t>Flexible Coupling, Clamping Type</t>
-  </si>
-  <si>
     <t>Vacuum Pad with Adaptor (8mm Diameter, M5 Female Thread)</t>
   </si>
   <si>
@@ -235,9 +184,6 @@
     <t>Wantai Stepper Motor 42BYGHW609, NEMA17, 1.8 deg/step</t>
   </si>
   <si>
-    <t>Required</t>
-  </si>
-  <si>
     <t>JLC PCB</t>
   </si>
   <si>
@@ -299,6 +245,87 @@
   </si>
   <si>
     <t>DS3115MG Servo</t>
+  </si>
+  <si>
+    <t>https://moduasm.co.za/product/2040-v-slot-1mtr-black-v-2040-1-b/</t>
+  </si>
+  <si>
+    <t>https://moduasm.co.za/product/2020-v-slot-1mtr-black-v-2020-1-b/</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/linear-rail-block-mgn12h-long.html</t>
+  </si>
+  <si>
+    <t>Linear Rail Block, MGN12H (Long)</t>
+  </si>
+  <si>
+    <t>Linear Rail, MGN12 x 1000mm with MGN12H Block</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/linear-rail-mgn12-x-1000mm-with-mgn12h-block.html</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/linear-chromed-steel-rod-8mm-1000mm.html</t>
+  </si>
+  <si>
+    <t>Linear chromed steel rod, 8mm, 1000mm</t>
+  </si>
+  <si>
+    <t>Linear bearing, LM8UU</t>
+  </si>
+  <si>
+    <t>Lead Screw nut, 8mm, Delrin</t>
+  </si>
+  <si>
+    <t>Modular Assembly Technology SA</t>
+  </si>
+  <si>
+    <t>Pulley, GT2, 20 Teeth for 6mm Belt</t>
+  </si>
+  <si>
+    <t>20 x 20mm Aluminium V-Slot Profile, 1m</t>
+  </si>
+  <si>
+    <t>20 x 40mm Aluminium V-Slot Profile, 1m</t>
+  </si>
+  <si>
+    <t>Timing Belt, GT2, 6mm wide, 1m long</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/pulley-gt2-20-teeth-for-6mm-belt.html</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/timing-belt-gt2-6mm-wide-1m-long-polyurethane.html</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/pillow-block-bearing-8mm-kp08.html</t>
+  </si>
+  <si>
+    <t>Pillow Block Bearing, 8mm, KP08</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/rigid-coupling-clamping-type.html</t>
+  </si>
+  <si>
+    <t>Rigid coupling, Clamping Type</t>
+  </si>
+  <si>
+    <t>https://www.diyelectronics.co.za/store/pulleys/1086-smooth-idler-pulley-3mm-bore-6mm-belt.html</t>
+  </si>
+  <si>
+    <t>Smooth Idler Pulley (3mm bore, 6mm belt)</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/linear-bearing-lm8uu-1-pair.html</t>
+  </si>
+  <si>
+    <t>https://www.3dprintingstore.co.za/centurionstore/lead-screw-nut-8mm-delrin.html</t>
+  </si>
+  <si>
+    <t>Components to be Purchased (Personal Funds)</t>
+  </si>
+  <si>
+    <t>Components to be Purchased (University Funds)</t>
   </si>
 </sst>
 </file>
@@ -416,7 +443,47 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="45">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -437,14 +504,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -455,37 +514,48 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -512,6 +582,43 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -526,8 +633,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FBB9695-A93A-472D-AB09-D0A262F94F20}" name="Table2" displayName="Table2" ref="A4:I27" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A4:I26" xr:uid="{1FBB9695-A93A-472D-AB09-D0A262F94F20}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93799A4D-F7D0-4428-9E5A-F36BAA1003ED}" name="Table22" displayName="Table22" ref="A4:I17" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A4:I16" xr:uid="{1FBB9695-A93A-472D-AB09-D0A262F94F20}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -539,33 +646,53 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5CB77036-6EDC-4C6E-AA7A-A24A28E76F4C}" name="Item description" totalsRowLabel="Total" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{FCAC24A4-9102-4758-9937-C980D10B8D1D}" name="Manufacturer" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{52A05EA1-8300-4387-B125-D38875D97D8E}" name="Manufacturer model number" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{ECE27936-736C-4CFF-A647-CD71A598E679}" name="Store" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{4AF6CAD2-FC5A-465A-B729-4B3E153A6B59}" name="Availability" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{CACCC691-E59B-4854-9A69-C610500DA6C2}" name="Quantity" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{40077FE9-E87F-44AF-ACCB-DC4EF8B152B1}" name="Unit price" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{8E3C7A3D-5684-421B-9B35-B72A3E3493EB}" name="Overall price" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7">
+    <tableColumn id="1" xr3:uid="{224B8563-CA28-4830-8DAC-378740C138E5}" name="Item description" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D06F58B9-4E86-4723-88AE-85F3AEA059CE}" name="Manufacturer" dataDxfId="25" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{FFBF4DF3-941A-4695-A39C-1F11BC1BCBBB}" name="Manufacturer model number" dataDxfId="24" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{73CDBACC-D763-452F-A065-93831D424856}" name="Store" dataDxfId="23" totalsRowDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{1871BA96-E5F4-46D5-8851-635B59D19BFF}" name="Availability" dataDxfId="22" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4D580AAB-B31A-4C9F-B194-01B895175E97}" name="Quantity" dataDxfId="21" totalsRowDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{DAF5B8E5-231A-493E-9CB7-F157A5C6EEFE}" name="Unit price" dataDxfId="20" totalsRowDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{CE933C0E-81AF-4600-9CB8-7B3C7B6D4AA5}" name="Overall price" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="10">
       <calculatedColumnFormula>PRODUCT(F5:G5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A381D153-A3F4-4955-9FC0-F2A8E888F576}" name="Source link" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{DC775C4B-9403-49AA-BA90-06A87D8EDE83}" name="Source link" dataDxfId="18" totalsRowDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C74F352E-5766-48C3-82D9-DC692DF5932E}" name="Table225" displayName="Table225" ref="A20:I35" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A20:I34" xr:uid="{C74F352E-5766-48C3-82D9-DC692DF5932E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{9439447C-397D-4058-A508-60D7594A3C16}" name="Item description" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{03E4D23C-B039-4643-955B-0DF67E8368FC}" name="Manufacturer" dataDxfId="34" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D3727F21-ED08-432B-8101-E639AE41B973}" name="Manufacturer model number" dataDxfId="33" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{589FA182-2225-4502-9DEC-33ED76075A16}" name="Store" dataDxfId="32" totalsRowDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{E3EA510F-9C7B-4AE5-8698-2B68FB711242}" name="Availability" dataDxfId="31" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{87E226C0-1483-4A45-89EE-81733099D06A}" name="Quantity" dataDxfId="30" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BBCE8B97-6B3E-4945-A954-B5C0AA12C577}" name="Unit price" dataDxfId="29" totalsRowDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{2CC7358D-6F67-482B-AA48-67C08D65D647}" name="Overall price" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="1">
+      <calculatedColumnFormula>PRODUCT(F21:G21)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{2626CA67-01E9-429F-B680-A3C5502986F0}" name="Source link" dataDxfId="28" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C13" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A4:C13" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -833,11 +960,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12D25E3-19BB-4652-925A-A2C85F180570}">
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +972,7 @@
     <col min="1" max="1" width="56.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
@@ -856,12 +983,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,19 +1002,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
@@ -895,638 +1022,781 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>80</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
       </c>
       <c r="G5" s="4">
-        <v>99.95</v>
+        <v>87.36</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" ref="H5:H16" si="0">PRODUCT(F5:G5)</f>
-        <v>199.9</v>
+        <f t="shared" ref="H5:H6" si="0">PRODUCT(F5:G5)</f>
+        <v>174.72</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>80</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="4">
-        <v>169.95</v>
+        <v>175.63</v>
       </c>
       <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>509.84999999999997</v>
+        <v>351.26</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>59</v>
+        <v>1199.95</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <f>PRODUCT(F7:G7)</f>
+        <v>1199.95</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>49.95</v>
+        <v>279.95</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="0"/>
-        <v>99.9</v>
+        <f>PRODUCT(F8:G8)</f>
+        <v>279.95</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4">
-        <v>49.95</v>
+        <v>149</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
-        <v>699.30000000000007</v>
+        <f t="shared" ref="H9" si="1">PRODUCT(F9:G9)</f>
+        <v>149</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F10" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G10" s="4">
-        <v>14.95</v>
+        <v>39</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>89.699999999999989</v>
+        <f>PRODUCT(F10:G10)</f>
+        <v>78</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="4">
-        <v>49.95</v>
+        <v>119.95</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="0"/>
-        <v>99.9</v>
+        <f>PRODUCT(F11:G11)</f>
+        <v>119.95</v>
       </c>
       <c r="I11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="4">
-        <v>119</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="0"/>
-        <v>119</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>27</v>
+        <f>PRODUCT(F12:G12)</f>
+        <v>39.950000000000003</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13" s="4">
-        <v>74.95</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="0"/>
-        <v>74.95</v>
+        <f>PRODUCT(F13:G13)</f>
+        <v>119.85000000000001</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
       </c>
       <c r="G14" s="4">
-        <v>79.95</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="H14" s="4">
         <f>PRODUCT(F14:G14)</f>
-        <v>159.9</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="4">
-        <v>64.95</v>
+        <v>137.15</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="0"/>
-        <v>129.9</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>30</v>
+        <f>PRODUCT(F15:G15)</f>
+        <v>137.15</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4">
-        <v>39.950000000000003</v>
+        <v>242.39</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="0"/>
-        <v>79.900000000000006</v>
+        <f>PRODUCT(F16:G16)</f>
+        <v>242.39</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="3">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <f>SUBTOTAL(109,Table22[Overall price])</f>
+        <v>2912.0699999999997</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="G17" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="H17" s="4">
-        <f>PRODUCT(F17:G17)</f>
-        <v>39.799999999999997</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4">
-        <v>19.95</v>
-      </c>
-      <c r="H18" s="4">
-        <f>PRODUCT(F18:G18)</f>
-        <v>19.95</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="H19" s="4">
-        <f>PRODUCT(F19:G19)</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="4">
-        <v>60</v>
-      </c>
-      <c r="H20" s="4">
-        <f>PRODUCT(F20:G20)</f>
-        <v>60</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F21" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" s="4">
-        <v>10</v>
+        <v>49.95</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" ref="H21:H26" si="1">PRODUCT(F21:G21)</f>
-        <v>30</v>
-      </c>
-      <c r="I21" s="3"/>
+        <f>PRODUCT(F21:G21)</f>
+        <v>199.8</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <v>114.63</v>
+      </c>
+      <c r="H22" s="4">
+        <f>PRODUCT(F22:G22)</f>
+        <v>114.63</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4">
-        <v>137.15</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
-        <v>137.15</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F23" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" s="4">
-        <v>114.63</v>
+        <v>10</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
-        <v>114.63</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>17</v>
-      </c>
+        <f>PRODUCT(F23:G23)</f>
+        <v>30</v>
+      </c>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G24" s="4">
-        <v>242.39</v>
+        <v>49.95</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="1"/>
-        <v>242.39</v>
+        <f>PRODUCT(F24:G24)</f>
+        <v>199.8</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>46</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25" s="4">
-        <v>349</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="1"/>
-        <v>349</v>
+        <f>PRODUCT(F25:G25)</f>
+        <v>159.80000000000001</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="F26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="4">
-        <v>200</v>
+        <v>69.95</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="1"/>
-        <v>200</v>
+        <f>PRODUCT(F26:G26)</f>
+        <v>139.9</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
+      <c r="D27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4">
+        <v>44.95</v>
+      </c>
       <c r="H27" s="4">
-        <f>SUBTOTAL(109,Table2[Overall price])</f>
-        <v>3519.0200000000004</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
+        <f>PRODUCT(F27:G27)</f>
+        <v>89.9</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" ref="H28" si="2">PRODUCT(F28:G28)</f>
+        <v>119.85000000000001</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4</v>
+      </c>
+      <c r="G29" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" ref="H29:H34" si="3">PRODUCT(F29:G29)</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>19.95</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="3"/>
+        <v>19.95</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>60</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>349</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="3"/>
+        <v>349</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <v>200</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4">
+        <f>SUBTOTAL(109,Table225[Overall price])</f>
+        <v>1727.33</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I5" r:id="rId1" xr:uid="{A869F3DC-7AF4-471C-8A59-83F4EBA0F038}"/>
-    <hyperlink ref="I6" r:id="rId2" xr:uid="{0B34D34B-2F90-45A0-A60B-246F9C9521D1}"/>
-    <hyperlink ref="I7" r:id="rId3" xr:uid="{B6CADA37-DC30-44DC-B25E-48FFA4CECCC8}"/>
-    <hyperlink ref="I8" r:id="rId4" xr:uid="{FE7314F5-07D4-4E1C-83AD-99EA9A317C26}"/>
-    <hyperlink ref="I9" r:id="rId5" xr:uid="{5EC2DAAB-11DE-49B5-9788-721A20167435}"/>
-    <hyperlink ref="I10" r:id="rId6" xr:uid="{C9072684-5B31-46FC-B864-AFBB63656077}"/>
-    <hyperlink ref="I11" r:id="rId7" xr:uid="{25C36732-1EBB-41E1-AF48-9247B8B17872}"/>
-    <hyperlink ref="I12" r:id="rId8" xr:uid="{98B0A240-B484-49B9-A321-AAB9F5882907}"/>
-    <hyperlink ref="I13" r:id="rId9" xr:uid="{950C062A-E1F6-4EA7-AE6B-C5B997B6E9A5}"/>
-    <hyperlink ref="I14" r:id="rId10" xr:uid="{682CA533-6AB7-49C5-B9A7-D81658EC798E}"/>
-    <hyperlink ref="I15" r:id="rId11" xr:uid="{58C0FE7F-40B1-482F-A297-9498498F0A4B}"/>
-    <hyperlink ref="I16" r:id="rId12" xr:uid="{9D6A88C2-9BD1-43D9-99E5-F55CC8BA18B1}"/>
-    <hyperlink ref="I22" r:id="rId13" xr:uid="{B0399635-4141-4733-BEDE-84C9E07C5F9E}"/>
-    <hyperlink ref="I23" r:id="rId14" xr:uid="{19CDA096-69A8-496B-A738-634F364621F2}"/>
-    <hyperlink ref="I24" r:id="rId15" xr:uid="{537BF3C1-76F7-4892-972F-1CF646ED0469}"/>
-    <hyperlink ref="I17" r:id="rId16" xr:uid="{E61937CC-C61C-470A-888E-22589590AA4C}"/>
-    <hyperlink ref="I25" r:id="rId17" xr:uid="{1DF0B828-FEFB-4DE4-88C8-0D95E6ADC11E}"/>
-    <hyperlink ref="I26" r:id="rId18" xr:uid="{92BC8783-EFB5-4E77-87BC-CC8EFF783D42}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{7381FD2B-B8A5-4F72-94E1-FB50D814874D}"/>
+    <hyperlink ref="I28" r:id="rId1" xr:uid="{67AA3613-E672-40FA-B23A-7A8C40805009}"/>
+    <hyperlink ref="I11" r:id="rId2" xr:uid="{6004BDB3-F660-4955-905B-9ACFD50B9FC1}"/>
+    <hyperlink ref="I12" r:id="rId3" xr:uid="{2254D1EC-AD4E-42A8-B22F-785D00FE3D81}"/>
+    <hyperlink ref="I16" r:id="rId4" xr:uid="{39643DEB-AB57-4712-ABDB-284351CA6DFE}"/>
+    <hyperlink ref="I22" r:id="rId5" xr:uid="{2683C246-C35C-4F93-8C38-61718A6C2759}"/>
+    <hyperlink ref="I15" r:id="rId6" xr:uid="{62221445-3A2F-4B25-8134-A23989F20E7F}"/>
+    <hyperlink ref="I29" r:id="rId7" xr:uid="{D6F1B62D-CA68-419B-9A4B-384E43A57191}"/>
+    <hyperlink ref="I32" r:id="rId8" xr:uid="{FCB72FC0-1500-4224-A6FB-6FD33566DABF}"/>
+    <hyperlink ref="I33" r:id="rId9" xr:uid="{9682A7ED-ACB6-4D24-858E-969A5B5D9581}"/>
+    <hyperlink ref="I34" r:id="rId10" xr:uid="{098BA267-63BB-4881-8A70-F3FA091CF08F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
-  <tableParts count="1">
-    <tablePart r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <tableParts count="2">
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1548,12 +1818,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,109 +1831,109 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>66</v>
+      <c r="C8" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
+      <c r="C9" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>66</v>
+      <c r="C10" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>66</v>
+      <c r="C11" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>66</v>
+      <c r="C12" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>66</v>
+      <c r="C13" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lab book to 13 August 2021
</commit_message>
<xml_diff>
--- a/proposal/budget.xlsx
+++ b/proposal/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - GE\Documents\University of Pretoria\Modules\Year 4 Semester 1\EPR 402\2021_conroy_ch\proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42776AC1-9134-4A04-827B-593067993FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C04428D-A03D-4B47-8913-B737DB9845DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Be Purchased" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
   <si>
     <t>Item description</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Source link</t>
   </si>
   <si>
-    <t>V-Slot Wheel Kit, Solid, Delrin</t>
-  </si>
-  <si>
     <t>Eccentric Nut for V-Wheels</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>https://za.rs-online.com/web/p/products/8368941/</t>
   </si>
   <si>
-    <t>https://www.3dprintingstore.co.za/centurionstore/v-slot-wheel-kit-solid-delrin.html</t>
-  </si>
-  <si>
     <t>https://www.3dprintingstore.co.za/centurionstore/eccentric-nut-for-v-wheels.html</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t>Overall price</t>
   </si>
   <si>
-    <t>2-3 working days delivery</t>
-  </si>
-  <si>
     <t>https://www.diyelectronics.co.za/store/limit-switches-probes/29-mechanical-limit-switch.html?search_query=limit&amp;results=250</t>
   </si>
   <si>
@@ -326,6 +317,12 @@
   </si>
   <si>
     <t>Components to be Purchased (University Funds)</t>
+  </si>
+  <si>
+    <t>https://www.diyelectronics.co.za/store/idler-wheels/1858-delrin-solid-v-wheel-with-625zz-bearing.html</t>
+  </si>
+  <si>
+    <t>Delrin Solid V-Wheel</t>
   </si>
 </sst>
 </file>
@@ -474,35 +471,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -532,33 +500,48 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -583,19 +566,33 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -646,53 +643,53 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{224B8563-CA28-4830-8DAC-378740C138E5}" name="Item description" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{D06F58B9-4E86-4723-88AE-85F3AEA059CE}" name="Manufacturer" dataDxfId="25" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{FFBF4DF3-941A-4695-A39C-1F11BC1BCBBB}" name="Manufacturer model number" dataDxfId="24" totalsRowDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{73CDBACC-D763-452F-A065-93831D424856}" name="Store" dataDxfId="23" totalsRowDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{1871BA96-E5F4-46D5-8851-635B59D19BFF}" name="Availability" dataDxfId="22" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{4D580AAB-B31A-4C9F-B194-01B895175E97}" name="Quantity" dataDxfId="21" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{DAF5B8E5-231A-493E-9CB7-F157A5C6EEFE}" name="Unit price" dataDxfId="20" totalsRowDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{CE933C0E-81AF-4600-9CB8-7B3C7B6D4AA5}" name="Overall price" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="10">
+    <tableColumn id="1" xr3:uid="{224B8563-CA28-4830-8DAC-378740C138E5}" name="Item description" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{D06F58B9-4E86-4723-88AE-85F3AEA059CE}" name="Manufacturer" dataDxfId="41" totalsRowDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{FFBF4DF3-941A-4695-A39C-1F11BC1BCBBB}" name="Manufacturer model number" dataDxfId="40" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{73CDBACC-D763-452F-A065-93831D424856}" name="Store" dataDxfId="39" totalsRowDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{1871BA96-E5F4-46D5-8851-635B59D19BFF}" name="Availability" dataDxfId="38" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{4D580AAB-B31A-4C9F-B194-01B895175E97}" name="Quantity" dataDxfId="37" totalsRowDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{DAF5B8E5-231A-493E-9CB7-F157A5C6EEFE}" name="Unit price" dataDxfId="36" totalsRowDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{CE933C0E-81AF-4600-9CB8-7B3C7B6D4AA5}" name="Overall price" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="19">
       <calculatedColumnFormula>PRODUCT(F5:G5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DC775C4B-9403-49AA-BA90-06A87D8EDE83}" name="Source link" dataDxfId="18" totalsRowDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{DC775C4B-9403-49AA-BA90-06A87D8EDE83}" name="Source link" dataDxfId="34" totalsRowDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C74F352E-5766-48C3-82D9-DC692DF5932E}" name="Table225" displayName="Table225" ref="A20:I35" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C74F352E-5766-48C3-82D9-DC692DF5932E}" name="Table225" displayName="Table225" ref="A20:I35" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A20:I34" xr:uid="{C74F352E-5766-48C3-82D9-DC692DF5932E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9439447C-397D-4058-A508-60D7594A3C16}" name="Item description" totalsRowLabel="Total" dataDxfId="35" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{03E4D23C-B039-4643-955B-0DF67E8368FC}" name="Manufacturer" dataDxfId="34" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D3727F21-ED08-432B-8101-E639AE41B973}" name="Manufacturer model number" dataDxfId="33" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{589FA182-2225-4502-9DEC-33ED76075A16}" name="Store" dataDxfId="32" totalsRowDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{E3EA510F-9C7B-4AE5-8698-2B68FB711242}" name="Availability" dataDxfId="31" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{87E226C0-1483-4A45-89EE-81733099D06A}" name="Quantity" dataDxfId="30" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{BBCE8B97-6B3E-4945-A954-B5C0AA12C577}" name="Unit price" dataDxfId="29" totalsRowDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{2CC7358D-6F67-482B-AA48-67C08D65D647}" name="Overall price" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{9439447C-397D-4058-A508-60D7594A3C16}" name="Item description" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{03E4D23C-B039-4643-955B-0DF67E8368FC}" name="Manufacturer" dataDxfId="16" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D3727F21-ED08-432B-8101-E639AE41B973}" name="Manufacturer model number" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{589FA182-2225-4502-9DEC-33ED76075A16}" name="Store" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{E3EA510F-9C7B-4AE5-8698-2B68FB711242}" name="Availability" dataDxfId="13" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{87E226C0-1483-4A45-89EE-81733099D06A}" name="Quantity" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BBCE8B97-6B3E-4945-A954-B5C0AA12C577}" name="Unit price" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{2CC7358D-6F67-482B-AA48-67C08D65D647}" name="Overall price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="1">
       <calculatedColumnFormula>PRODUCT(F21:G21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2626CA67-01E9-429F-B680-A3C5502986F0}" name="Source link" dataDxfId="28" totalsRowDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{2626CA67-01E9-429F-B680-A3C5502986F0}" name="Source link" dataDxfId="9" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C13" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}" name="Table3" displayName="Table3" ref="A4:C13" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A4:C13" xr:uid="{E676303D-D7F6-4AF8-9833-7BA1F064A504}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{FF8EC5F8-A61D-4260-8AAE-9D3D3F4994D9}" name="Item description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{11041A41-E042-448D-9F3C-0673B4090205}" name="Quantity" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{A46BFDCC-C92B-4ED4-84D2-09C68DD80DFC}" name="Status" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -961,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12D25E3-19BB-4652-925A-A2C85F180570}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,12 +980,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,19 +999,19 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
@@ -1022,15 +1019,15 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3">
         <v>2</v>
@@ -1043,20 +1040,20 @@
         <v>174.72</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3">
         <v>2</v>
@@ -1069,18 +1066,18 @@
         <v>351.26</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F7" s="3">
         <v>1</v>
@@ -1093,20 +1090,20 @@
         <v>1199.95</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="3">
         <v>1</v>
@@ -1119,20 +1116,20 @@
         <v>279.95</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F9" s="3">
         <v>1</v>
@@ -1145,20 +1142,20 @@
         <v>149</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F10" s="3">
         <v>2</v>
@@ -1167,24 +1164,24 @@
         <v>39</v>
       </c>
       <c r="H10" s="4">
-        <f>PRODUCT(F10:G10)</f>
+        <f t="shared" ref="H10:H16" si="2">PRODUCT(F10:G10)</f>
         <v>78</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -1193,22 +1190,22 @@
         <v>119.95</v>
       </c>
       <c r="H11" s="4">
-        <f>PRODUCT(F11:G11)</f>
+        <f t="shared" si="2"/>
         <v>119.95</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
@@ -1217,24 +1214,24 @@
         <v>39.950000000000003</v>
       </c>
       <c r="H12" s="4">
-        <f>PRODUCT(F12:G12)</f>
+        <f t="shared" si="2"/>
         <v>39.950000000000003</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F13" s="3">
         <v>3</v>
@@ -1243,24 +1240,24 @@
         <v>39.950000000000003</v>
       </c>
       <c r="H13" s="4">
-        <f>PRODUCT(F13:G13)</f>
+        <f t="shared" si="2"/>
         <v>119.85000000000001</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F14" s="3">
         <v>2</v>
@@ -1269,28 +1266,28 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="H14" s="4">
-        <f>PRODUCT(F14:G14)</f>
+        <f t="shared" si="2"/>
         <v>19.899999999999999</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3">
         <v>1</v>
@@ -1299,28 +1296,28 @@
         <v>137.15</v>
       </c>
       <c r="H15" s="4">
-        <f>PRODUCT(F15:G15)</f>
+        <f t="shared" si="2"/>
         <v>137.15</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1329,16 +1326,16 @@
         <v>242.39</v>
       </c>
       <c r="H16" s="4">
-        <f>PRODUCT(F16:G16)</f>
+        <f t="shared" si="2"/>
         <v>242.39</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1354,7 +1351,7 @@
     </row>
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1368,19 +1365,19 @@
         <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>4</v>
@@ -1388,45 +1385,45 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F21" s="3">
         <v>4</v>
       </c>
       <c r="G21" s="4">
-        <v>49.95</v>
+        <v>59.95</v>
       </c>
       <c r="H21" s="4">
         <f>PRODUCT(F21:G21)</f>
-        <v>199.8</v>
+        <v>239.8</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" s="3">
         <v>1</v>
@@ -1435,24 +1432,24 @@
         <v>114.63</v>
       </c>
       <c r="H22" s="4">
-        <f>PRODUCT(F22:G22)</f>
+        <f t="shared" ref="H22:H27" si="3">PRODUCT(F22:G22)</f>
         <v>114.63</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F23" s="3">
         <v>3</v>
@@ -1461,22 +1458,22 @@
         <v>10</v>
       </c>
       <c r="H23" s="4">
-        <f>PRODUCT(F23:G23)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F24" s="3">
         <v>4</v>
@@ -1485,24 +1482,24 @@
         <v>49.95</v>
       </c>
       <c r="H24" s="4">
-        <f>PRODUCT(F24:G24)</f>
+        <f t="shared" si="3"/>
         <v>199.8</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F25" s="3">
         <v>4</v>
@@ -1511,24 +1508,24 @@
         <v>39.950000000000003</v>
       </c>
       <c r="H25" s="4">
-        <f>PRODUCT(F25:G25)</f>
+        <f t="shared" si="3"/>
         <v>159.80000000000001</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
@@ -1537,24 +1534,24 @@
         <v>69.95</v>
       </c>
       <c r="H26" s="4">
-        <f>PRODUCT(F26:G26)</f>
+        <f t="shared" si="3"/>
         <v>139.9</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F27" s="3">
         <v>2</v>
@@ -1563,50 +1560,50 @@
         <v>44.95</v>
       </c>
       <c r="H27" s="4">
-        <f>PRODUCT(F27:G27)</f>
+        <f t="shared" si="3"/>
         <v>89.9</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F28" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" s="4">
         <v>39.950000000000003</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" ref="H28" si="2">PRODUCT(F28:G28)</f>
-        <v>119.85000000000001</v>
+        <f t="shared" ref="H28" si="4">PRODUCT(F28:G28)</f>
+        <v>159.80000000000001</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F29" s="3">
         <v>4</v>
@@ -1615,28 +1612,28 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" ref="H29:H34" si="3">PRODUCT(F29:G29)</f>
+        <f t="shared" ref="H29:H34" si="5">PRODUCT(F29:G29)</f>
         <v>39.799999999999997</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -1645,24 +1642,24 @@
         <v>19.95</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19.95</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -1671,28 +1668,28 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.9000000000000004</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1701,26 +1698,26 @@
         <v>60</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
@@ -1729,24 +1726,24 @@
         <v>349</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>349</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
@@ -1755,16 +1752,16 @@
         <v>200</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1774,11 +1771,11 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4">
         <f>SUBTOTAL(109,Table225[Overall price])</f>
-        <v>1727.33</v>
+        <v>1807.28</v>
       </c>
       <c r="I35" s="3"/>
     </row>
-    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I28" r:id="rId1" xr:uid="{67AA3613-E672-40FA-B23A-7A8C40805009}"/>
@@ -1791,12 +1788,16 @@
     <hyperlink ref="I32" r:id="rId8" xr:uid="{FCB72FC0-1500-4224-A6FB-6FD33566DABF}"/>
     <hyperlink ref="I33" r:id="rId9" xr:uid="{9682A7ED-ACB6-4D24-858E-969A5B5D9581}"/>
     <hyperlink ref="I34" r:id="rId10" xr:uid="{098BA267-63BB-4881-8A70-F3FA091CF08F}"/>
+    <hyperlink ref="I10" r:id="rId11" xr:uid="{928E97C6-1790-4230-AB08-C1DC9E48811B}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{D2F48930-A49D-46C2-853D-5B8311AD82E7}"/>
+    <hyperlink ref="I24" r:id="rId13" xr:uid="{A4EF4FB0-13CD-4C5C-85F9-C21A7C13DF90}"/>
+    <hyperlink ref="I21" r:id="rId14" xr:uid="{C12A1484-EC48-4FE1-99B8-DCB326895562}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="2">
-    <tablePart r:id="rId12"/>
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1805,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E588218-957E-4AA9-A72D-F3B084945E29}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,12 +1819,12 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1831,109 +1832,109 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>